<commit_message>
change status in excel
</commit_message>
<xml_diff>
--- a/Lab6_testcase.xlsx
+++ b/Lab6_testcase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansu\Downloads\lab6_SQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA\Lab6\SQA_lab6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C5F63E-F0B7-467D-A8BC-1915F7ECF6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E75AB85-223C-4BDE-8E93-D9645CAC4652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{05E5A71A-1B0B-AF41-826B-8255904D086F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="123">
   <si>
     <t>Condition</t>
   </si>
@@ -405,13 +405,16 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>No run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -496,6 +499,19 @@
       <color theme="1"/>
       <name val="TH Sarabun New"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="TH SarabunPSK"/>
+      <family val="2"/>
+      <charset val="222"/>
     </font>
   </fonts>
   <fills count="5">
@@ -625,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -787,11 +803,47 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF92D050"/>
@@ -3666,8 +3718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDA246C7-2BD6-B342-8D0F-04BB389B0A44}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="C30" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4811,9 +4863,8 @@
       <c r="J37" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="K37" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>Pass</v>
+      <c r="K37" s="58" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -4830,6 +4881,17 @@
     <mergeCell ref="A7:A8"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="K9:K37">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4839,8 +4901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC61237-DA71-1543-BDB0-22C4D3E98B73}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5590,9 +5652,8 @@
       <c r="G33" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="H33" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Pass</v>
+      <c r="H33" s="57" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -5615,9 +5676,8 @@
       <c r="G34" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="H34" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Pass</v>
+      <c r="H34" s="57" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="27" x14ac:dyDescent="0.25">
@@ -5640,9 +5700,8 @@
       <c r="G35" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="H35" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>Pass</v>
+      <c r="H35" s="57" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -5660,10 +5719,10 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="H9:H35">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>